<commit_message>
Completely reworked file import, issue was not with file input, issue was with AttributeType declaration. Now deliberately creating files within the application hierarchy, will implement deletion to remove initial dataset from hierarchy such that only anonymized, safe data may be accessed if anything attempted
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5160"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="5">
   <si>
     <t>age</t>
   </si>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -873,11 +873,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -906,13 +906,24 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
       </c>
       <c r="C5">
         <v>81675</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>43</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>81931</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -970,14 +981,25 @@
         <v>81931</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>70</v>
+      </c>
+      <c r="B16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16">
+        <v>81931</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
         <v>45</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>3</v>
       </c>
-      <c r="C17">
+      <c r="C18">
         <v>81931</v>
       </c>
     </row>

</xml_diff>